<commit_message>
Perbaikan Semua (profile, stok, detail, detail penjualan)
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102798ED-48E0-4DF8-988F-E6439B292DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445BE868-FD09-414F-96D0-E693A5107580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C15C43D8-397C-4B8A-A760-E47E32667305}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7810" xr2:uid="{C15C43D8-397C-4B8A-A760-E47E32667305}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>kategori_id</t>
   </si>
@@ -51,10 +51,16 @@
     <t>harga_jual</t>
   </si>
   <si>
-    <t>Telur Omega(10 butir)</t>
-  </si>
-  <si>
-    <t>ABCD</t>
+    <t>BJU01</t>
+  </si>
+  <si>
+    <t>Baju tidur bunga</t>
+  </si>
+  <si>
+    <t>CLN01</t>
+  </si>
+  <si>
+    <t>Celana jeans kulot</t>
   </si>
 </sst>
 </file>
@@ -417,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6A4900-E57A-44B9-BE3B-463B50144AA0}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,16 +460,33 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2">
         <v>22000</v>
       </c>
       <c r="E2">
         <v>25000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>145000</v>
+      </c>
+      <c r="E3">
+        <v>175000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>